<commit_message>
Crime Rates By Region: Adding Map
</commit_message>
<xml_diff>
--- a/data/Crime_In_US_By_Region/Crime_In_US_By_Region_2016.xlsx
+++ b/data/Crime_In_US_By_Region/Crime_In_US_By_Region_2016.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{8F823B19-3A05-924C-A8C5-0012FC61B98F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6ADFEB5-DDF6-E84C-BF1D-BC237A88088A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="5400" windowWidth="25600" windowHeight="15540"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="16tbl02" sheetId="1" r:id="rId1"/>
@@ -14,15 +14,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'16tbl02'!$A$1:$Q$14</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'16tbl02'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="152511" fullCalcOnLoad="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -92,41 +84,41 @@
     <t>Population</t>
   </si>
   <si>
+    <t>Murder and nonnegligent manslaughter Rate per 100,000</t>
+  </si>
+  <si>
+    <t>Rape</t>
+  </si>
+  <si>
+    <t>Rape Rate per 100,000</t>
+  </si>
+  <si>
+    <t>Robbery Rate per 100,000</t>
+  </si>
+  <si>
+    <t>Aggravated assault Rate per 100,000</t>
+  </si>
+  <si>
+    <t>Burglary Rate per 100,000</t>
+  </si>
+  <si>
+    <t>Larceny-theft Rate per 100,000</t>
+  </si>
+  <si>
+    <t>Motor vehicle theft Rate per 100,000</t>
+  </si>
+  <si>
     <t>Murder and nonnegligent manslaughter</t>
-  </si>
-  <si>
-    <t>Murder and nonnegligent manslaughter Rate per 100,000</t>
-  </si>
-  <si>
-    <t>Rape</t>
-  </si>
-  <si>
-    <t>Rape Rate per 100,000</t>
-  </si>
-  <si>
-    <t>Robbery Rate per 100,000</t>
-  </si>
-  <si>
-    <t>Aggravated assault Rate per 100,000</t>
-  </si>
-  <si>
-    <t>Burglary Rate per 100,000</t>
-  </si>
-  <si>
-    <t>Larceny-theft Rate per 100,000</t>
-  </si>
-  <si>
-    <t>Motor vehicle theft Rate per 100,000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="171" formatCode="#,##0.0\ "/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0\ "/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -136,6 +128,7 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -235,7 +228,7 @@
     <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -247,13 +240,13 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="171" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -594,11 +587,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q14" sqref="A1:Q14"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -634,46 +627,46 @@
         <v>20</v>
       </c>
       <c r="D1" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="7" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>24</v>
       </c>
       <c r="H1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J1" s="7" t="s">
         <v>2</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="N1" s="7" t="s">
         <v>4</v>
       </c>
       <c r="O1" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="P1" s="7" t="s">
         <v>5</v>
       </c>
       <c r="Q1" s="7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:17" s="4" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">

</xml_diff>